<commit_message>
Edit Screen information and guide v1.7.5
- Edit Leak/Pressure unit.
- disable export cal. date to report.
- edit 7.4L format.
- add label guide before/after testing and under create report process.
- disable clear tbSN after click btnClear
</commit_message>
<xml_diff>
--- a/Leak/ext_Resources/7.4kW_CCU_L.xlsx
+++ b/Leak/ext_Resources/7.4kW_CCU_L.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSharpe-Leak\Leak\ext_Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnonymouS\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D319C-6DDE-4C01-A040-A8C4E5712A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F75FE08-80DA-4E3B-8F1F-5900EC1A5826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>:</t>
   </si>
@@ -212,13 +212,16 @@
     <t>-0.1 to 0.4</t>
   </si>
   <si>
-    <t>Cal. Due Date:</t>
-  </si>
-  <si>
     <t>ECD17020028</t>
   </si>
   <si>
     <t>QTS_LEAK_00_ECD170200xx_BMW_CCU_7.4kW_large</t>
+  </si>
+  <si>
+    <t>BMW_CCU_large 7.4kW</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
 </sst>
 </file>
@@ -615,10 +618,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="188" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -649,15 +648,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,6 +665,19 @@
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="188" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" shrinkToFit="1"/>
@@ -704,7 +707,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{E7171E97-7E30-41EB-9543-03E2A3EA6934}"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1077,23 +1080,23 @@
   </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>15875</xdr:colOff>
+      <xdr:colOff>112778</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1101,7 +1104,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1109,14 +1112,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="17312" t="19791" r="9189" b="19785"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3057525" y="7585075"/>
-          <a:ext cx="2387600" cy="1857375"/>
+          <a:off x="2686050" y="7572375"/>
+          <a:ext cx="2855978" cy="1866899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1456,23 +1458,23 @@
   </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
+      <xdr:colOff>103253</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
+        <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA43F771-4E2A-49E7-B8CF-8294DE0D4832}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1480,7 +1482,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1488,14 +1490,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="17312" t="19791" r="9189" b="19785"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3086100" y="7572375"/>
-          <a:ext cx="2387600" cy="1857375"/>
+          <a:off x="2676525" y="7572375"/>
+          <a:ext cx="2855978" cy="1866899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1885,7 +1886,7 @@
   <dimension ref="A1:AS270"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AT19" sqref="AT19"/>
+      <selection activeCell="AT48" sqref="AT48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2047,7 +2048,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="86" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K6" s="86"/>
       <c r="L6" s="86"/>
@@ -2063,7 +2064,9 @@
       <c r="V6" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="89"/>
+      <c r="W6" s="89" t="s">
+        <v>59</v>
+      </c>
       <c r="X6" s="89"/>
       <c r="Y6" s="89"/>
       <c r="Z6" s="89"/>
@@ -2101,31 +2104,33 @@
       <c r="I7" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="68" t="s">
+      <c r="J7" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
       <c r="S7" s="63"/>
       <c r="T7" s="63"/>
       <c r="U7" s="63"/>
       <c r="V7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="90"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
-      <c r="AB7" s="68"/>
-      <c r="AC7" s="68"/>
-      <c r="AD7" s="68"/>
+      <c r="W7" s="90" t="s">
+        <v>60</v>
+      </c>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AG7" s="63"/>
@@ -2156,29 +2161,29 @@
       <c r="I8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
       <c r="S8" s="63"/>
       <c r="T8" s="63"/>
       <c r="U8" s="63"/>
       <c r="V8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
-      <c r="Z8" s="68"/>
-      <c r="AA8" s="68"/>
-      <c r="AB8" s="68"/>
-      <c r="AC8" s="68"/>
-      <c r="AD8" s="68"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
@@ -2187,12 +2192,12 @@
       <c r="AJ8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AK8" s="69"/>
-      <c r="AL8" s="69"/>
-      <c r="AM8" s="69"/>
-      <c r="AN8" s="69"/>
-      <c r="AO8" s="69"/>
-      <c r="AP8" s="69"/>
+      <c r="AK8" s="68"/>
+      <c r="AL8" s="68"/>
+      <c r="AM8" s="68"/>
+      <c r="AN8" s="68"/>
+      <c r="AO8" s="68"/>
+      <c r="AP8" s="68"/>
       <c r="AQ8" s="14"/>
     </row>
     <row r="9" spans="1:43" s="5" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2357,9 +2362,7 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
-      <c r="AG12" s="65" t="s">
-        <v>57</v>
-      </c>
+      <c r="AG12" s="65"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
@@ -2407,14 +2410,12 @@
       <c r="AD13" s="24"/>
       <c r="AE13" s="24"/>
       <c r="AF13" s="24"/>
-      <c r="AG13" s="66">
-        <v>44231</v>
-      </c>
-      <c r="AH13" s="66"/>
-      <c r="AI13" s="66"/>
-      <c r="AJ13" s="66"/>
-      <c r="AK13" s="66"/>
-      <c r="AL13" s="66"/>
+      <c r="AG13" s="85"/>
+      <c r="AH13" s="85"/>
+      <c r="AI13" s="85"/>
+      <c r="AJ13" s="85"/>
+      <c r="AK13" s="85"/>
+      <c r="AL13" s="85"/>
       <c r="AM13" s="25"/>
       <c r="AN13" s="25"/>
       <c r="AO13" s="4"/>
@@ -2721,7 +2722,7 @@
       <c r="L20" s="27"/>
       <c r="M20" s="27"/>
       <c r="N20" s="59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O20" s="59"/>
       <c r="P20" s="59"/>
@@ -3507,159 +3508,159 @@
     </row>
     <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="71" t="s">
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
-      <c r="U37" s="72"/>
-      <c r="V37" s="72"/>
-      <c r="W37" s="72"/>
-      <c r="X37" s="72"/>
-      <c r="Y37" s="72"/>
-      <c r="Z37" s="72"/>
-      <c r="AA37" s="72"/>
-      <c r="AB37" s="72"/>
-      <c r="AC37" s="72"/>
-      <c r="AD37" s="72"/>
-      <c r="AE37" s="72"/>
-      <c r="AF37" s="72"/>
-      <c r="AG37" s="72"/>
-      <c r="AH37" s="72"/>
-      <c r="AI37" s="72"/>
-      <c r="AJ37" s="72"/>
-      <c r="AK37" s="72"/>
-      <c r="AL37" s="72"/>
-      <c r="AM37" s="72"/>
-      <c r="AN37" s="72"/>
-      <c r="AO37" s="72"/>
-      <c r="AP37" s="73"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="71"/>
+      <c r="U37" s="71"/>
+      <c r="V37" s="71"/>
+      <c r="W37" s="71"/>
+      <c r="X37" s="71"/>
+      <c r="Y37" s="71"/>
+      <c r="Z37" s="71"/>
+      <c r="AA37" s="71"/>
+      <c r="AB37" s="71"/>
+      <c r="AC37" s="71"/>
+      <c r="AD37" s="71"/>
+      <c r="AE37" s="71"/>
+      <c r="AF37" s="71"/>
+      <c r="AG37" s="71"/>
+      <c r="AH37" s="71"/>
+      <c r="AI37" s="71"/>
+      <c r="AJ37" s="71"/>
+      <c r="AK37" s="71"/>
+      <c r="AL37" s="71"/>
+      <c r="AM37" s="71"/>
+      <c r="AN37" s="71"/>
+      <c r="AO37" s="71"/>
+      <c r="AP37" s="72"/>
       <c r="AQ37" s="33"/>
     </row>
     <row r="38" spans="1:45" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="74" t="s">
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="P38" s="75"/>
-      <c r="Q38" s="75"/>
-      <c r="R38" s="75"/>
-      <c r="S38" s="75"/>
-      <c r="T38" s="76"/>
-      <c r="U38" s="74" t="s">
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="74"/>
+      <c r="S38" s="74"/>
+      <c r="T38" s="75"/>
+      <c r="U38" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="V38" s="75"/>
-      <c r="W38" s="75"/>
-      <c r="X38" s="75"/>
-      <c r="Y38" s="75"/>
-      <c r="Z38" s="75"/>
-      <c r="AA38" s="76"/>
-      <c r="AB38" s="77" t="s">
+      <c r="V38" s="74"/>
+      <c r="W38" s="74"/>
+      <c r="X38" s="74"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="74"/>
+      <c r="AA38" s="75"/>
+      <c r="AB38" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="AC38" s="75"/>
-      <c r="AD38" s="75"/>
-      <c r="AE38" s="75"/>
-      <c r="AF38" s="75"/>
-      <c r="AG38" s="76"/>
-      <c r="AH38" s="78" t="s">
+      <c r="AC38" s="74"/>
+      <c r="AD38" s="74"/>
+      <c r="AE38" s="74"/>
+      <c r="AF38" s="74"/>
+      <c r="AG38" s="75"/>
+      <c r="AH38" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="AI38" s="79"/>
-      <c r="AJ38" s="79"/>
-      <c r="AK38" s="79"/>
-      <c r="AL38" s="79"/>
-      <c r="AM38" s="70" t="s">
+      <c r="AI38" s="84"/>
+      <c r="AJ38" s="84"/>
+      <c r="AK38" s="84"/>
+      <c r="AL38" s="84"/>
+      <c r="AM38" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AN38" s="70"/>
-      <c r="AO38" s="70"/>
-      <c r="AP38" s="70"/>
+      <c r="AN38" s="69"/>
+      <c r="AO38" s="69"/>
+      <c r="AP38" s="69"/>
       <c r="AQ38" s="33"/>
     </row>
     <row r="39" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="81"/>
-      <c r="O39" s="81" t="s">
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="P39" s="81"/>
-      <c r="Q39" s="81"/>
-      <c r="R39" s="81"/>
-      <c r="S39" s="81"/>
-      <c r="T39" s="81"/>
-      <c r="U39" s="81" t="s">
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="77"/>
+      <c r="S39" s="77"/>
+      <c r="T39" s="77"/>
+      <c r="U39" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="V39" s="81"/>
-      <c r="W39" s="81"/>
-      <c r="X39" s="81"/>
-      <c r="Y39" s="81"/>
-      <c r="Z39" s="81"/>
-      <c r="AA39" s="81"/>
-      <c r="AB39" s="82" t="s">
+      <c r="V39" s="77"/>
+      <c r="W39" s="77"/>
+      <c r="X39" s="77"/>
+      <c r="Y39" s="77"/>
+      <c r="Z39" s="77"/>
+      <c r="AA39" s="77"/>
+      <c r="AB39" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="AC39" s="83"/>
-      <c r="AD39" s="83"/>
-      <c r="AE39" s="83"/>
-      <c r="AF39" s="83"/>
-      <c r="AG39" s="83"/>
-      <c r="AH39" s="84"/>
-      <c r="AI39" s="85"/>
-      <c r="AJ39" s="85"/>
-      <c r="AK39" s="85"/>
-      <c r="AL39" s="85"/>
-      <c r="AM39" s="67" t="s">
+      <c r="AC39" s="79"/>
+      <c r="AD39" s="79"/>
+      <c r="AE39" s="79"/>
+      <c r="AF39" s="79"/>
+      <c r="AG39" s="79"/>
+      <c r="AH39" s="80"/>
+      <c r="AI39" s="81"/>
+      <c r="AJ39" s="81"/>
+      <c r="AK39" s="81"/>
+      <c r="AL39" s="81"/>
+      <c r="AM39" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="AN39" s="67"/>
-      <c r="AO39" s="67"/>
-      <c r="AP39" s="67"/>
+      <c r="AN39" s="66"/>
+      <c r="AO39" s="66"/>
+      <c r="AP39" s="66"/>
       <c r="AQ39" s="33"/>
     </row>
     <row r="40" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4607,14 +4608,13 @@
     <row r="270" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="AH39:AL39"/>
+    <mergeCell ref="AG13:AL13"/>
     <mergeCell ref="J6:R6"/>
     <mergeCell ref="AK6:AP6"/>
     <mergeCell ref="J7:R7"/>
     <mergeCell ref="AK7:AP7"/>
     <mergeCell ref="W6:AD6"/>
     <mergeCell ref="W7:AD7"/>
-    <mergeCell ref="AG13:AL13"/>
     <mergeCell ref="AM39:AP39"/>
     <mergeCell ref="J8:R8"/>
     <mergeCell ref="AK8:AP8"/>
@@ -4622,14 +4622,15 @@
     <mergeCell ref="O37:AP37"/>
     <mergeCell ref="O38:T38"/>
     <mergeCell ref="U38:AA38"/>
+    <mergeCell ref="B39:N39"/>
+    <mergeCell ref="O39:T39"/>
+    <mergeCell ref="U39:AA39"/>
+    <mergeCell ref="AB39:AG39"/>
+    <mergeCell ref="AH39:AL39"/>
     <mergeCell ref="AB38:AG38"/>
     <mergeCell ref="AH38:AL38"/>
     <mergeCell ref="AM38:AP38"/>
     <mergeCell ref="W8:AD8"/>
-    <mergeCell ref="B39:N39"/>
-    <mergeCell ref="O39:T39"/>
-    <mergeCell ref="U39:AA39"/>
-    <mergeCell ref="AB39:AG39"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" sqref="M28 G28:K28" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
@@ -4747,7 +4748,7 @@
   <dimension ref="A1:AS270"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AU43" sqref="AU43"/>
+      <selection activeCell="W8" sqref="W8:AD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4905,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="86" t="str">
-        <f>Cooling!J6</f>
+        <f>Cooling!$J$6</f>
         <v>ECD17020028</v>
       </c>
       <c r="K6" s="86"/>
@@ -4919,7 +4920,10 @@
       <c r="V6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W6" s="86"/>
+      <c r="W6" s="86" t="str">
+        <f>Cooling!$W$6</f>
+        <v>BMW_CCU_large 7.4kW</v>
+      </c>
       <c r="X6" s="86"/>
       <c r="Y6" s="86"/>
       <c r="Z6" s="86"/>
@@ -4953,29 +4957,32 @@
       <c r="I7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="68" t="str">
-        <f>Cooling!J7</f>
+      <c r="J7" s="67" t="str">
+        <f>Cooling!$J$7</f>
         <v>BMW</v>
       </c>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="68"/>
-      <c r="N7" s="68"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="68"/>
-      <c r="Q7" s="68"/>
-      <c r="R7" s="68"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="67"/>
+      <c r="P7" s="67"/>
+      <c r="Q7" s="67"/>
+      <c r="R7" s="67"/>
       <c r="V7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W7" s="68"/>
-      <c r="X7" s="68"/>
-      <c r="Y7" s="68"/>
-      <c r="Z7" s="68"/>
-      <c r="AA7" s="68"/>
-      <c r="AB7" s="68"/>
-      <c r="AC7" s="68"/>
-      <c r="AD7" s="68"/>
+      <c r="W7" s="67" t="str">
+        <f>Cooling!$W$7</f>
+        <v>C1</v>
+      </c>
+      <c r="X7" s="67"/>
+      <c r="Y7" s="67"/>
+      <c r="Z7" s="67"/>
+      <c r="AA7" s="67"/>
+      <c r="AB7" s="67"/>
+      <c r="AC7" s="67"/>
+      <c r="AD7" s="67"/>
       <c r="AE7" s="11"/>
       <c r="AF7" s="11"/>
       <c r="AH7" s="11"/>
@@ -5005,26 +5012,26 @@
       <c r="I8" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-      <c r="R8" s="68"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
       <c r="V8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="W8" s="68"/>
-      <c r="X8" s="68"/>
-      <c r="Y8" s="68"/>
-      <c r="Z8" s="68"/>
-      <c r="AA8" s="68"/>
-      <c r="AB8" s="68"/>
-      <c r="AC8" s="68"/>
-      <c r="AD8" s="68"/>
+      <c r="W8" s="67"/>
+      <c r="X8" s="67"/>
+      <c r="Y8" s="67"/>
+      <c r="Z8" s="67"/>
+      <c r="AA8" s="67"/>
+      <c r="AB8" s="67"/>
+      <c r="AC8" s="67"/>
+      <c r="AD8" s="67"/>
       <c r="AE8" s="11"/>
       <c r="AF8" s="11"/>
       <c r="AG8" s="11"/>
@@ -5033,12 +5040,12 @@
       <c r="AJ8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AK8" s="69"/>
-      <c r="AL8" s="69"/>
-      <c r="AM8" s="69"/>
-      <c r="AN8" s="69"/>
-      <c r="AO8" s="69"/>
-      <c r="AP8" s="69"/>
+      <c r="AK8" s="68"/>
+      <c r="AL8" s="68"/>
+      <c r="AM8" s="68"/>
+      <c r="AN8" s="68"/>
+      <c r="AO8" s="68"/>
+      <c r="AP8" s="68"/>
       <c r="AQ8" s="14"/>
     </row>
     <row r="9" spans="1:43" s="5" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -5200,9 +5207,7 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="3"/>
       <c r="AF12" s="3"/>
-      <c r="AG12" s="65" t="s">
-        <v>57</v>
-      </c>
+      <c r="AG12" s="65"/>
       <c r="AM12" s="4"/>
       <c r="AN12" s="4"/>
       <c r="AO12" s="4"/>
@@ -5250,14 +5255,12 @@
       <c r="AD13" s="24"/>
       <c r="AE13" s="24"/>
       <c r="AF13" s="24"/>
-      <c r="AG13" s="66">
-        <v>44231</v>
-      </c>
-      <c r="AH13" s="66"/>
-      <c r="AI13" s="66"/>
-      <c r="AJ13" s="66"/>
-      <c r="AK13" s="66"/>
-      <c r="AL13" s="66"/>
+      <c r="AG13" s="85"/>
+      <c r="AH13" s="85"/>
+      <c r="AI13" s="85"/>
+      <c r="AJ13" s="85"/>
+      <c r="AK13" s="85"/>
+      <c r="AL13" s="85"/>
       <c r="AM13" s="25"/>
       <c r="AN13" s="25"/>
       <c r="AO13" s="4"/>
@@ -6337,157 +6340,157 @@
     </row>
     <row r="37" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="31"/>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="71" t="s">
+      <c r="C37" s="69"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="69"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="P37" s="72"/>
-      <c r="Q37" s="72"/>
-      <c r="R37" s="72"/>
-      <c r="S37" s="72"/>
-      <c r="T37" s="72"/>
-      <c r="U37" s="72"/>
-      <c r="V37" s="72"/>
-      <c r="W37" s="72"/>
-      <c r="X37" s="72"/>
-      <c r="Y37" s="72"/>
-      <c r="Z37" s="72"/>
-      <c r="AA37" s="72"/>
-      <c r="AB37" s="72"/>
-      <c r="AC37" s="72"/>
-      <c r="AD37" s="72"/>
-      <c r="AE37" s="72"/>
-      <c r="AF37" s="72"/>
-      <c r="AG37" s="72"/>
-      <c r="AH37" s="72"/>
-      <c r="AI37" s="72"/>
-      <c r="AJ37" s="72"/>
-      <c r="AK37" s="72"/>
-      <c r="AL37" s="72"/>
-      <c r="AM37" s="72"/>
-      <c r="AN37" s="72"/>
-      <c r="AO37" s="72"/>
-      <c r="AP37" s="73"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="71"/>
+      <c r="R37" s="71"/>
+      <c r="S37" s="71"/>
+      <c r="T37" s="71"/>
+      <c r="U37" s="71"/>
+      <c r="V37" s="71"/>
+      <c r="W37" s="71"/>
+      <c r="X37" s="71"/>
+      <c r="Y37" s="71"/>
+      <c r="Z37" s="71"/>
+      <c r="AA37" s="71"/>
+      <c r="AB37" s="71"/>
+      <c r="AC37" s="71"/>
+      <c r="AD37" s="71"/>
+      <c r="AE37" s="71"/>
+      <c r="AF37" s="71"/>
+      <c r="AG37" s="71"/>
+      <c r="AH37" s="71"/>
+      <c r="AI37" s="71"/>
+      <c r="AJ37" s="71"/>
+      <c r="AK37" s="71"/>
+      <c r="AL37" s="71"/>
+      <c r="AM37" s="71"/>
+      <c r="AN37" s="71"/>
+      <c r="AO37" s="71"/>
+      <c r="AP37" s="72"/>
       <c r="AQ37" s="33"/>
     </row>
     <row r="38" spans="1:45" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="31"/>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="70"/>
-      <c r="E38" s="70"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="70"/>
-      <c r="H38" s="70"/>
-      <c r="I38" s="70"/>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="74" t="s">
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="P38" s="75"/>
-      <c r="Q38" s="75"/>
-      <c r="R38" s="75"/>
-      <c r="S38" s="75"/>
-      <c r="T38" s="76"/>
-      <c r="U38" s="74" t="s">
+      <c r="P38" s="74"/>
+      <c r="Q38" s="74"/>
+      <c r="R38" s="74"/>
+      <c r="S38" s="74"/>
+      <c r="T38" s="75"/>
+      <c r="U38" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="V38" s="75"/>
-      <c r="W38" s="75"/>
-      <c r="X38" s="75"/>
-      <c r="Y38" s="75"/>
-      <c r="Z38" s="75"/>
-      <c r="AA38" s="76"/>
-      <c r="AB38" s="74" t="s">
+      <c r="V38" s="74"/>
+      <c r="W38" s="74"/>
+      <c r="X38" s="74"/>
+      <c r="Y38" s="74"/>
+      <c r="Z38" s="74"/>
+      <c r="AA38" s="75"/>
+      <c r="AB38" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="AC38" s="75"/>
-      <c r="AD38" s="75"/>
-      <c r="AE38" s="75"/>
-      <c r="AF38" s="75"/>
-      <c r="AG38" s="76"/>
-      <c r="AH38" s="78" t="s">
+      <c r="AC38" s="74"/>
+      <c r="AD38" s="74"/>
+      <c r="AE38" s="74"/>
+      <c r="AF38" s="74"/>
+      <c r="AG38" s="75"/>
+      <c r="AH38" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="AI38" s="79"/>
-      <c r="AJ38" s="79"/>
-      <c r="AK38" s="79"/>
-      <c r="AL38" s="79"/>
-      <c r="AM38" s="70" t="s">
+      <c r="AI38" s="84"/>
+      <c r="AJ38" s="84"/>
+      <c r="AK38" s="84"/>
+      <c r="AL38" s="84"/>
+      <c r="AM38" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AN38" s="70"/>
-      <c r="AO38" s="70"/>
-      <c r="AP38" s="70"/>
+      <c r="AN38" s="69"/>
+      <c r="AO38" s="69"/>
+      <c r="AP38" s="69"/>
       <c r="AQ38" s="33"/>
     </row>
     <row r="39" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81"/>
-      <c r="I39" s="81"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="81"/>
-      <c r="N39" s="81"/>
-      <c r="O39" s="81" t="s">
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="77"/>
+      <c r="N39" s="77"/>
+      <c r="O39" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="P39" s="81"/>
-      <c r="Q39" s="81"/>
-      <c r="R39" s="81"/>
-      <c r="S39" s="81"/>
-      <c r="T39" s="81"/>
-      <c r="U39" s="81" t="s">
+      <c r="P39" s="77"/>
+      <c r="Q39" s="77"/>
+      <c r="R39" s="77"/>
+      <c r="S39" s="77"/>
+      <c r="T39" s="77"/>
+      <c r="U39" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="V39" s="81"/>
-      <c r="W39" s="81"/>
-      <c r="X39" s="81"/>
-      <c r="Y39" s="81"/>
-      <c r="Z39" s="81"/>
-      <c r="AA39" s="81"/>
-      <c r="AB39" s="82" t="s">
+      <c r="V39" s="77"/>
+      <c r="W39" s="77"/>
+      <c r="X39" s="77"/>
+      <c r="Y39" s="77"/>
+      <c r="Z39" s="77"/>
+      <c r="AA39" s="77"/>
+      <c r="AB39" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="AC39" s="83"/>
-      <c r="AD39" s="83"/>
-      <c r="AE39" s="83"/>
-      <c r="AF39" s="83"/>
-      <c r="AG39" s="83"/>
+      <c r="AC39" s="79"/>
+      <c r="AD39" s="79"/>
+      <c r="AE39" s="79"/>
+      <c r="AF39" s="79"/>
+      <c r="AG39" s="79"/>
       <c r="AH39" s="91"/>
       <c r="AI39" s="91"/>
       <c r="AJ39" s="91"/>
       <c r="AK39" s="91"/>
       <c r="AL39" s="91"/>
-      <c r="AM39" s="67"/>
-      <c r="AN39" s="67"/>
-      <c r="AO39" s="67"/>
-      <c r="AP39" s="67"/>
+      <c r="AM39" s="66"/>
+      <c r="AN39" s="66"/>
+      <c r="AO39" s="66"/>
+      <c r="AP39" s="66"/>
       <c r="AQ39" s="33"/>
     </row>
     <row r="40" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>